<commit_message>
Ajustes graficos // se agrega el excel de pruebas
</commit_message>
<xml_diff>
--- a/public/prueba.xlsx
+++ b/public/prueba.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA470F9E-39F1-4219-950C-48062F108B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>primer apellido</t>
   </si>
@@ -75,12 +76,6 @@
     <t>Moreno</t>
   </si>
   <si>
-    <t>Torres</t>
-  </si>
-  <si>
-    <t>Leandro</t>
-  </si>
-  <si>
     <t>Esteban</t>
   </si>
   <si>
@@ -96,9 +91,6 @@
     <t>prueba@gmail.com</t>
   </si>
   <si>
-    <t>cl 25 s 10 11</t>
-  </si>
-  <si>
     <t>Correo Electronico</t>
   </si>
   <si>
@@ -108,35 +100,49 @@
     <t>Si</t>
   </si>
   <si>
-    <t>Vega</t>
-  </si>
-  <si>
-    <t>Herrera</t>
-  </si>
-  <si>
-    <t>Jenny</t>
-  </si>
-  <si>
     <t>Prueba</t>
   </si>
   <si>
-    <t>123857@gmail.com</t>
-  </si>
-  <si>
-    <t>cl 25 s 10 12</t>
-  </si>
-  <si>
     <t>#</t>
+  </si>
+  <si>
+    <t>calle 19 1 10</t>
+  </si>
+  <si>
+    <t>prueba@uniandes.edu.co</t>
+  </si>
+  <si>
+    <t>Jeimy</t>
+  </si>
+  <si>
+    <t>Vergara</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Pineda</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -159,13 +165,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -193,7 +202,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -471,18 +480,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -544,49 +553,49 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2">
+        <v>1023935749</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="G2">
-        <v>1023915749</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
       </c>
       <c r="K2">
         <v>3195904684</v>
       </c>
       <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" t="s">
-        <v>28</v>
-      </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -594,55 +603,58 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="D3" t="s">
-        <v>31</v>
-      </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>1023915749</v>
       </c>
       <c r="H3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="K3">
         <v>3175904644</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="Q3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J3" r:id="rId1" xr:uid="{D339FAC0-D2E3-4F12-ABA7-7D6162174A4D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>